<commit_message>
Included Jira ID for each test case data.
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteDOCS/testdata/DocumentRegistryTestData-Newtransmittal-Subsite.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteDOCS/testdata/DocumentRegistryTestData-Newtransmittal-Subsite.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\suiteDOCS\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS_Sprint5\Fulcrum_FluidTX_Trunk\src\com\proj\suiteDOCS\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>To</t>
   </si>
@@ -96,19 +96,31 @@
     <t>Issued for Review</t>
   </si>
   <si>
-    <t>Comments for Issued for Review</t>
-  </si>
-  <si>
     <t>Request for Information</t>
   </si>
   <si>
-    <t>Comments for Request for Information</t>
-  </si>
-  <si>
     <t>Issued for Approval</t>
   </si>
   <si>
     <t>Approved</t>
+  </si>
+  <si>
+    <t>RefID</t>
+  </si>
+  <si>
+    <t>LATFLD-77</t>
+  </si>
+  <si>
+    <t>LATFLD-76</t>
+  </si>
+  <si>
+    <t>LATFLD-75</t>
+  </si>
+  <si>
+    <t>LATFLD-22</t>
+  </si>
+  <si>
+    <t>Submission</t>
   </si>
 </sst>
 </file>
@@ -509,198 +521,218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="28.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.85546875" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="27" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>16</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>24</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>17</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>19</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
         <v>25</v>
       </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="4" spans="1:16">
-      <c r="A4" t="s">
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F5" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G5" t="s">
         <v>16</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H5" t="s">
         <v>26</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J5" t="s">
         <v>17</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N5" t="s">
         <v>19</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O5" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" t="s">
-        <v>19</v>
-      </c>
-      <c r="N5" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" display="https://leapthought.atlassian.net/browse/LATFLD-77"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://leapthought.atlassian.net/browse/LATFLD-76"/>
+    <hyperlink ref="A2" r:id="rId3" display="https://leapthought.atlassian.net/browse/LATFLD-75"/>
+  </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated message with <currentPage> of <totalPages>.
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteDOCS/testdata/DocumentRegistryTestData-Newtransmittal-Subsite.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteDOCS/testdata/DocumentRegistryTestData-Newtransmittal-Subsite.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS_Sprint5\Fulcrum_FluidTX_Trunk\src\com\proj\suiteDOCS\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_S5_NR\Fulcrum_FluidTX_Trunk\src\com\proj\suiteDOCS\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Transmittals_New" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>To</t>
   </si>
@@ -78,9 +78,6 @@
     <t>IssueReason</t>
   </si>
   <si>
-    <t>Message for New transmittal</t>
-  </si>
-  <si>
     <t>Issued for Information</t>
   </si>
   <si>
@@ -121,6 +118,12 @@
   </si>
   <si>
     <t>Submission</t>
+  </si>
+  <si>
+    <t>Message for New transmittal - subsite</t>
+  </si>
+  <si>
+    <t>Mes</t>
   </si>
 </sst>
 </file>
@@ -521,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -540,19 +543,21 @@
     <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="27" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="27" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" customWidth="1"/>
+    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -591,24 +596,27 @@
         <v>4</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
@@ -620,24 +628,28 @@
         <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="N2" t="s">
-        <v>19</v>
+      <c r="N2" t="str">
+        <f>CONCATENATE(ROW()-1," of ",COUNTA(A2:A100)," ",O2)</f>
+        <v>1 of 4 Message for New transmittal - subsite</v>
+      </c>
+      <c r="O2" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -649,27 +661,31 @@
         <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J3" t="s">
         <v>17</v>
       </c>
-      <c r="N3" t="s">
-        <v>19</v>
+      <c r="N3" t="str">
+        <f>CONCATENATE(ROW()-1," of ",COUNTA(A2:A100)," ",O2)</f>
+        <v>2 of 4 Message for New transmittal - subsite</v>
       </c>
       <c r="O3" t="s">
         <v>33</v>
       </c>
+      <c r="P3" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -681,27 +697,31 @@
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s">
         <v>17</v>
       </c>
-      <c r="N4" t="s">
-        <v>19</v>
+      <c r="N4" t="str">
+        <f>CONCATENATE(ROW()-1," of ",COUNTA(A2:A100)," ",O2)</f>
+        <v>3 of 4 Message for New transmittal - subsite</v>
       </c>
       <c r="O4" t="s">
         <v>33</v>
       </c>
+      <c r="P4" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -713,16 +733,20 @@
         <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J5" t="s">
         <v>17</v>
       </c>
-      <c r="N5" t="s">
-        <v>19</v>
+      <c r="N5" t="str">
+        <f>CONCATENATE(ROW()-1," of ",COUNTA(A2:A100)," ",O2)</f>
+        <v>4 of 4 Message for New transmittal - subsite</v>
       </c>
       <c r="O5" t="s">
-        <v>27</v>
+        <v>33</v>
+      </c>
+      <c r="P5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>